<commit_message>
se arreglaron las fnciones falta la de horarios
</commit_message>
<xml_diff>
--- a/uploads/2902081.xlsx
+++ b/uploads/2902081.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AVA\serverbienestar\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97137FC-3630-41CC-8A97-5B842691A34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ACB6E8-47F8-459E-8E15-00D92A7F0D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -698,49 +698,49 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1049,33 +1049,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
     <col min="4" max="4" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="59"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -1141,7 +1141,7 @@
       <c r="A5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="11"/>
@@ -1159,7 +1159,7 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="50"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1175,7 +1175,7 @@
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1191,7 +1191,7 @@
       <c r="A8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="51"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
@@ -1207,7 +1207,7 @@
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="51" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="11"/>
@@ -1227,7 +1227,7 @@
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="12"/>
       <c r="D10" s="1" t="s">
         <v>14</v>
@@ -1245,7 +1245,7 @@
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="3"/>
       <c r="D11" s="7" t="s">
         <v>9</v>
@@ -1263,7 +1263,7 @@
       <c r="A12" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="48"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="31"/>
       <c r="D12" s="30" t="s">
         <v>12</v>
@@ -1305,7 +1305,7 @@
       <c r="A14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="51" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="13"/>
@@ -1325,7 +1325,7 @@
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="12"/>
       <c r="D15" s="1" t="s">
         <v>14</v>
@@ -1343,7 +1343,7 @@
       <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="3"/>
       <c r="D16" s="7" t="s">
         <v>9</v>
@@ -1361,7 +1361,7 @@
       <c r="A17" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="48"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="31"/>
       <c r="D17" s="30" t="s">
         <v>12</v>
@@ -1376,22 +1376,22 @@
       <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="54"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="56"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="57" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1413,7 +1413,7 @@
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="47"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="7" t="s">
         <v>9</v>
       </c>
@@ -1453,7 +1453,7 @@
       <c r="A22" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="48"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="35" t="s">
         <v>21</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="A23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="57" t="s">
         <v>46</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1497,7 +1497,7 @@
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="50"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
@@ -1519,7 +1519,7 @@
       <c r="A25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="50"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="7" t="s">
         <v>9</v>
       </c>
@@ -1541,7 +1541,7 @@
       <c r="A26" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="51"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="35" t="s">
         <v>21</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="A28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="57" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1609,7 +1609,7 @@
       <c r="A29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="50"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="5" t="s">
         <v>18</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="A30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="50"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="7" t="s">
         <v>9</v>
       </c>
@@ -1653,7 +1653,7 @@
       <c r="A31" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="51"/>
+      <c r="B31" s="50"/>
       <c r="C31" s="35" t="s">
         <v>21</v>
       </c>
@@ -1672,22 +1672,22 @@
       <c r="H31" s="36"/>
     </row>
     <row r="32" spans="1:8" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="54"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="56"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="57" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="13"/>
@@ -1701,7 +1701,7 @@
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="50"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
@@ -1713,7 +1713,7 @@
       <c r="A35" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="50"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1725,7 +1725,7 @@
       <c r="A36" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="50"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="31"/>
@@ -1737,7 +1737,7 @@
       <c r="A37" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="59" t="s">
         <v>49</v>
       </c>
       <c r="C37" s="17"/>
@@ -1751,7 +1751,7 @@
       <c r="A38" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="55"/>
+      <c r="B38" s="59"/>
       <c r="C38" s="38"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
@@ -1763,7 +1763,7 @@
       <c r="A39" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="55"/>
+      <c r="B39" s="59"/>
       <c r="C39" s="18"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -1775,7 +1775,7 @@
       <c r="A40" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="56"/>
+      <c r="B40" s="60"/>
       <c r="C40" s="40"/>
       <c r="D40" s="41"/>
       <c r="E40" s="41"/>
@@ -1786,20 +1786,15 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="49"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:H18"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="C41:H41"/>
     <mergeCell ref="B23:B26"/>
@@ -1807,6 +1802,11 @@
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>